<commit_message>
cardData v2, create list
</commit_message>
<xml_diff>
--- a/기획/카드 데이터1차 .xlsx
+++ b/기획/카드 데이터1차 .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4045166b326961f7/바탕 화면/워오카/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\War_of_Card\기획\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{ED4695F0-3670-41A1-BE2B-F24388B66786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DC913D9-326B-4D35-A4D3-EAE76B133345}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B3F1DC-223B-438D-A041-87C04792798C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="0" windowWidth="17496" windowHeight="12240" activeTab="1" xr2:uid="{CA7A336F-C6E9-493E-8055-0C6AAE6B3B3E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{CA7A336F-C6E9-493E-8055-0C6AAE6B3B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="커맨더" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -388,10 +386,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -697,15 +691,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="18.59765625" customWidth="1"/>
-    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.19921875" customWidth="1"/>
-    <col min="5" max="5" width="79.09765625" customWidth="1"/>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.8125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -713,13 +707,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -730,10 +724,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -747,17 +741,17 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="21.09765625" customWidth="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
     <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="14.19921875" customWidth="1"/>
+    <col min="6" max="6" width="14.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -791,7 +785,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -808,7 +802,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -825,7 +819,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B5" t="s">
         <v>25</v>
       </c>
@@ -842,7 +836,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B6" t="s">
         <v>26</v>
       </c>
@@ -859,7 +853,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -876,7 +870,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -893,7 +887,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B9" t="s">
         <v>33</v>
       </c>
@@ -910,7 +904,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B12" t="s">
         <v>37</v>
       </c>
@@ -926,16 +920,16 @@
   <dimension ref="B1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="13.19921875" customWidth="1"/>
-    <col min="4" max="4" width="105.296875" customWidth="1"/>
+    <col min="2" max="2" width="13.1875" customWidth="1"/>
+    <col min="4" max="4" width="105.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.6">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -957,7 +951,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.6">
       <c r="B3" t="s">
         <v>13</v>
       </c>

</xml_diff>